<commit_message>
Adding a function to apply TableStyle to Excel module
</commit_message>
<xml_diff>
--- a/pyRevitMEP.tab/Lab.panel/Excel.pushbutton/ImportExportTemplate.xlsx
+++ b/pyRevitMEP.tab/Lab.panel/Excel.pushbutton/ImportExportTemplate.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18431"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\FichiersLocauxRevit\pyRevitMEP.extension\pyRevitMEP.tab\Lab.panel\Excel.pushbutton\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\FichiersLocauxRevit\pyRevitMEP\pyRevitMEP.extension\pyRevitMEP.tab\Lab.panel\Excel.pushbutton\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -25,8 +25,22 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="3">
+  <si>
+    <t>Service</t>
+  </si>
+  <si>
+    <t>Local</t>
+  </si>
+  <si>
+    <t>Remarque</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -73,6 +87,18 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tableau1" displayName="Tableau1" ref="A1:C14" totalsRowShown="0">
+  <autoFilter ref="A1:C14"/>
+  <tableColumns count="3">
+    <tableColumn id="1" name="Service"/>
+    <tableColumn id="2" name="Local"/>
+    <tableColumn id="3" name="Remarque"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -372,36 +398,81 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="2" width="10.7109375" customWidth="1"/>
+    <col min="3" max="3" width="65.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updates to pyrevit 4.5 on lab part and lib
</commit_message>
<xml_diff>
--- a/pyRevitMEP.tab/Lab.panel/Excel.pushbutton/ImportExportTemplate.xlsx
+++ b/pyRevitMEP.tab/Lab.panel/Excel.pushbutton/ImportExportTemplate.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18431"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\FichiersLocauxRevit\pyRevitMEP\pyRevitMEP.extension\pyRevitMEP.tab\Lab.panel\Excel.pushbutton\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\FichiersLocauxRevit\pyRevitMEP.extension\pyRevitMEP.tab\Lab.panel\Excel.pushbutton\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -15,6 +15,7 @@
     <sheet name="SpaceCheck" sheetId="3" r:id="rId1"/>
     <sheet name="Import" sheetId="1" r:id="rId2"/>
     <sheet name="Export" sheetId="2" r:id="rId3"/>
+    <sheet name="ScriptError" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -475,4 +476,16 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Lab work and some PEP8 cleaning
</commit_message>
<xml_diff>
--- a/pyRevitMEP.tab/Lab.panel/Excel.pushbutton/ImportExportTemplate.xlsx
+++ b/pyRevitMEP.tab/Lab.panel/Excel.pushbutton/ImportExportTemplate.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18431"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\FichiersLocauxRevit\pyRevitMEP.extension\pyRevitMEP.tab\Lab.panel\Excel.pushbutton\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\FichiersLocauxRevit\pyRevitMEP\pyRevitMEP.extension\pyRevitMEP.tab\Lab.panel\Excel.pushbutton\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -17,7 +17,7 @@
     <sheet name="Export" sheetId="2" r:id="rId3"/>
     <sheet name="ScriptError" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="171027" calcMode="manual"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -402,13 +402,13 @@
   <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+      <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="10.7109375" customWidth="1"/>
-    <col min="3" max="3" width="65.7109375" customWidth="1"/>
+    <col min="3" max="3" width="80.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>